<commit_message>
before merge dayhighdd to master
</commit_message>
<xml_diff>
--- a/all_times/Rolling_monthly_reports/ all_times_Rolling_Monthly_Report_TR3000_DD3000_SZ1_DYN_False_TDDTrue.xlsx
+++ b/all_times/Rolling_monthly_reports/ all_times_Rolling_Monthly_Report_TR3000_DD3000_SZ1_DYN_False_TDDTrue.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liikurserv\PycharmProjects\1500_count\all_times\Rolling_monthly_reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D2D874-50EB-4295-9230-B24700881E28}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Rolling_months" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -313,8 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,14 +396,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -456,7 +442,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,27 +474,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -540,24 +508,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -733,19 +683,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -978,12 +926,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1207,7 +1155,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -1431,7 +1379,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" s="2" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
@@ -1595,7 +1543,7 @@
         <v>83.75</v>
       </c>
       <c r="BC5" s="2">
-        <v>77.540000000000006</v>
+        <v>77.54000000000001</v>
       </c>
       <c r="BD5" s="2">
         <v>71.94</v>
@@ -1655,7 +1603,7 @@
         <v>102.5</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78">
       <c r="A6" s="1" t="s">
         <v>81</v>
       </c>
@@ -1879,39 +1827,39 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B7">
-        <v>70.540000000000006</v>
+        <v>70.54000000000001</v>
       </c>
       <c r="C7">
-        <v>70.709999999999994</v>
+        <v>70.70999999999999</v>
       </c>
       <c r="D7">
-        <v>71.180000000000007</v>
+        <v>71.18000000000001</v>
       </c>
       <c r="E7">
         <v>71.78</v>
       </c>
       <c r="F7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="G7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="H7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="I7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="J7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="K7">
-        <v>72.040000000000006</v>
+        <v>72.04000000000001</v>
       </c>
       <c r="L7">
         <v>72.17</v>
@@ -1920,7 +1868,7 @@
         <v>72.47</v>
       </c>
       <c r="N7">
-        <v>72.459999999999994</v>
+        <v>72.45999999999999</v>
       </c>
       <c r="O7">
         <v>72.86</v>
@@ -1929,55 +1877,55 @@
         <v>73.42</v>
       </c>
       <c r="Q7">
-        <v>73.790000000000006</v>
+        <v>73.79000000000001</v>
       </c>
       <c r="R7">
-        <v>74.180000000000007</v>
+        <v>74.18000000000001</v>
       </c>
       <c r="S7">
-        <v>74.510000000000005</v>
+        <v>74.51000000000001</v>
       </c>
       <c r="T7">
-        <v>75.180000000000007</v>
+        <v>75.18000000000001</v>
       </c>
       <c r="U7">
-        <v>75.510000000000005</v>
+        <v>75.51000000000001</v>
       </c>
       <c r="V7">
         <v>75.09</v>
       </c>
       <c r="W7">
-        <v>74.989999999999995</v>
+        <v>74.98999999999999</v>
       </c>
       <c r="X7">
-        <v>75.150000000000006</v>
+        <v>75.15000000000001</v>
       </c>
       <c r="Y7">
-        <v>75.680000000000007</v>
+        <v>75.68000000000001</v>
       </c>
       <c r="Z7">
         <v>76.22</v>
       </c>
       <c r="AA7">
-        <v>76.930000000000007</v>
+        <v>76.93000000000001</v>
       </c>
       <c r="AB7">
         <v>77.77</v>
       </c>
       <c r="AC7">
-        <v>78.569999999999993</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="AD7">
         <v>79.3</v>
       </c>
       <c r="AE7">
-        <v>80.209999999999994</v>
+        <v>80.20999999999999</v>
       </c>
       <c r="AF7">
-        <v>81.069999999999993</v>
+        <v>81.06999999999999</v>
       </c>
       <c r="AG7">
-        <v>81.99</v>
+        <v>81.98999999999999</v>
       </c>
       <c r="AH7">
         <v>82.75</v>
@@ -1998,7 +1946,7 @@
         <v>85.98</v>
       </c>
       <c r="AN7">
-        <v>86.68</v>
+        <v>86.68000000000001</v>
       </c>
       <c r="AO7">
         <v>87.16</v>
@@ -2007,13 +1955,13 @@
         <v>88.13</v>
       </c>
       <c r="AQ7">
-        <v>89.24</v>
+        <v>89.23999999999999</v>
       </c>
       <c r="AR7">
         <v>90.23</v>
       </c>
       <c r="AS7">
-        <v>90.93</v>
+        <v>90.93000000000001</v>
       </c>
       <c r="AT7">
         <v>91.12</v>
@@ -2022,7 +1970,7 @@
         <v>91.62</v>
       </c>
       <c r="AV7">
-        <v>89.79</v>
+        <v>89.79000000000001</v>
       </c>
       <c r="AW7">
         <v>83.5</v>
@@ -2043,7 +1991,7 @@
         <v>48</v>
       </c>
       <c r="BC7">
-        <v>40.340000000000003</v>
+        <v>40.34</v>
       </c>
       <c r="BD7">
         <v>33.51</v>
@@ -2091,7 +2039,7 @@
         <v>31.8</v>
       </c>
       <c r="BS7">
-        <v>36.380000000000003</v>
+        <v>36.38</v>
       </c>
       <c r="BT7">
         <v>43.54</v>
@@ -2103,7 +2051,7 @@
         <v>7.94</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78">
       <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
@@ -2327,10 +2275,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -2566,7 +2514,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78">
       <c r="A11" s="1" t="s">
         <v>85</v>
       </c>
@@ -2802,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78">
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
@@ -3038,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -3274,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:78" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" s="3" customFormat="1">
       <c r="A14" s="1" t="s">
         <v>88</v>
       </c>
@@ -3282,13 +3230,13 @@
         <v>91.22</v>
       </c>
       <c r="C14" s="3">
-        <v>91.18</v>
+        <v>91.18000000000001</v>
       </c>
       <c r="D14" s="3">
-        <v>91.07</v>
+        <v>91.06999999999999</v>
       </c>
       <c r="E14" s="3">
-        <v>90.93</v>
+        <v>90.93000000000001</v>
       </c>
       <c r="F14" s="3">
         <v>91.61</v>
@@ -3303,10 +3251,10 @@
         <v>95.86</v>
       </c>
       <c r="J14" s="3">
-        <v>97.32</v>
+        <v>97.31999999999999</v>
       </c>
       <c r="K14" s="3">
-        <v>98.9</v>
+        <v>98.90000000000001</v>
       </c>
       <c r="L14" s="3">
         <v>100</v>
@@ -3498,12 +3446,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:78" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" s="4" customFormat="1">
       <c r="A15" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B15" s="4">
-        <v>8.7799999999999994</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="C15" s="4">
         <v>8.82</v>
@@ -3515,7 +3463,7 @@
         <v>9.07</v>
       </c>
       <c r="F15" s="4">
-        <v>8.39</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="G15" s="4">
         <v>7.06</v>
@@ -3524,13 +3472,13 @@
         <v>5.56</v>
       </c>
       <c r="I15" s="4">
-        <v>4.1399999999999997</v>
+        <v>4.14</v>
       </c>
       <c r="J15" s="4">
         <v>2.68</v>
       </c>
       <c r="K15" s="4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="L15" s="4">
         <v>0</v>
@@ -3722,12 +3670,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78">
       <c r="A16" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>91</v>
       </c>
@@ -3762,7 +3710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>92</v>
       </c>
@@ -3797,21 +3745,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B19">
-        <v>87.1</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="C19">
-        <v>87.1</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="D19">
-        <v>87.1</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="E19">
-        <v>87.1</v>
+        <v>87.09999999999999</v>
       </c>
       <c r="F19">
         <v>81</v>
@@ -3832,7 +3780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>94</v>
       </c>
@@ -3867,7 +3815,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>95</v>
       </c>
@@ -3900,11 +3848,6 @@
       </c>
       <c r="K21">
         <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>